<commit_message>
EPBDS-14346 Fix conversion when the argument type is String
</commit_message>
<xml_diff>
--- a/WSFrontend/org.openl.rules.ruleservice/test-resources/RulesFrontendTest/RulesFrontendTest/multimodule/Module3_1.xlsx
+++ b/WSFrontend/org.openl.rules.ruleservice/test-resources/RulesFrontendTest/RulesFrontendTest/multimodule/Module3_1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
   <si>
     <t>Method String worldHello(int hour)</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>return data;</t>
+  </si>
+  <si>
+    <t>Method String str2str(String data)</t>
   </si>
   <si>
     <t>Datatype Complex</t>
@@ -1410,7 +1413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1680,44 +1683,34 @@
     </row>
     <row r="32" ht="13.55" customHeight="1">
       <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
     </row>
     <row r="33" ht="13.55" customHeight="1">
-      <c r="A33" s="2"/>
-      <c r="B33" t="s" s="13">
+      <c r="A33" s="4"/>
+      <c r="B33" t="s" s="5">
         <v>17</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="7"/>
       <c r="E33" s="2"/>
     </row>
     <row r="34" ht="13.55" customHeight="1">
-      <c r="A34" s="2"/>
-      <c r="B34" t="s" s="13">
-        <v>18</v>
-      </c>
-      <c r="C34" t="s" s="13">
-        <v>19</v>
-      </c>
-      <c r="D34" t="s" s="13">
-        <v>20</v>
-      </c>
+      <c r="A34" s="4"/>
+      <c r="B34" t="s" s="8">
+        <v>16</v>
+      </c>
+      <c r="C34" s="9"/>
+      <c r="D34" s="7"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" ht="13.55" customHeight="1">
       <c r="A35" s="2"/>
-      <c r="B35" t="s" s="13">
-        <v>21</v>
-      </c>
-      <c r="C35" t="s" s="13">
-        <v>22</v>
-      </c>
-      <c r="D35" s="14">
-        <v>25</v>
-      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="2"/>
       <c r="E35" s="2"/>
     </row>
     <row r="36" ht="13.55" customHeight="1">
@@ -1727,8 +1720,50 @@
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
     </row>
+    <row r="37" ht="13.55" customHeight="1">
+      <c r="A37" s="2"/>
+      <c r="B37" t="s" s="13">
+        <v>18</v>
+      </c>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" ht="13.55" customHeight="1">
+      <c r="A38" s="2"/>
+      <c r="B38" t="s" s="13">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s" s="13">
+        <v>20</v>
+      </c>
+      <c r="D38" t="s" s="13">
+        <v>21</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" ht="13.55" customHeight="1">
+      <c r="A39" s="2"/>
+      <c r="B39" t="s" s="13">
+        <v>22</v>
+      </c>
+      <c r="C39" t="s" s="13">
+        <v>23</v>
+      </c>
+      <c r="D39" s="14">
+        <v>25</v>
+      </c>
+      <c r="E39" s="2"/>
+    </row>
+    <row r="40" ht="13.55" customHeight="1">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
@@ -1744,6 +1779,8 @@
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
EPBDS-14389 Implement tryJSON() method
</commit_message>
<xml_diff>
--- a/WSFrontend/org.openl.rules.ruleservice/test-resources/RulesFrontendTest/RulesFrontendTest/multimodule/Module3_1.xlsx
+++ b/WSFrontend/org.openl.rules.ruleservice/test-resources/RulesFrontendTest/RulesFrontendTest/multimodule/Module3_1.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="34">
   <si>
     <t>Method String worldHello(int hour)</t>
   </si>
@@ -83,6 +83,36 @@
   </si>
   <si>
     <t>age</t>
+  </si>
+  <si>
+    <t>SimpleRules String validate(State st)</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>= error("CA is not allowed")</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>= error("CD1", "Failure")</t>
+  </si>
+  <si>
+    <t>= error(new Complex("Yura", 1000))</t>
   </si>
 </sst>
 </file>
@@ -1413,7 +1443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1761,6 +1791,82 @@
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
+    </row>
+    <row r="41" ht="13.55" customHeight="1">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+    </row>
+    <row r="42" ht="13.55" customHeight="1">
+      <c r="A42" s="2"/>
+      <c r="B42" t="s" s="13">
+        <v>24</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" ht="13.55" customHeight="1">
+      <c r="A43" s="2"/>
+      <c r="B43" t="s" s="13">
+        <v>25</v>
+      </c>
+      <c r="C43" t="s" s="13">
+        <v>26</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" ht="13.55" customHeight="1">
+      <c r="A44" s="2"/>
+      <c r="B44" t="s" s="13">
+        <v>27</v>
+      </c>
+      <c r="C44" t="s" s="13">
+        <v>28</v>
+      </c>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" ht="13.55" customHeight="1">
+      <c r="A45" s="2"/>
+      <c r="B45" t="s" s="13">
+        <v>29</v>
+      </c>
+      <c r="C45" t="s" s="13">
+        <v>30</v>
+      </c>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+    </row>
+    <row r="46" ht="13.55" customHeight="1">
+      <c r="A46" s="2"/>
+      <c r="B46" t="s" s="13">
+        <v>31</v>
+      </c>
+      <c r="C46" t="s" s="13">
+        <v>32</v>
+      </c>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+    </row>
+    <row r="47" ht="13.55" customHeight="1">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" t="s" s="13">
+        <v>33</v>
+      </c>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+    </row>
+    <row r="48" ht="13.55" customHeight="1">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="17">

</xml_diff>